<commit_message>
updated csv for links per square, imagesper square and standard deviation column
</commit_message>
<xml_diff>
--- a/data/TopArticleUsage_Published_in_2021_JCO.xlsx
+++ b/data/TopArticleUsage_Published_in_2021_JCO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03e7a7648bc4d477/JACC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A91A2F61-A44F-6946-A4AB-C7A549E3152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A91A2F61-A44F-6946-A4AB-C7A549E3152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2C7C6EF-D055-3341-A72C-8198ADF7141B}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="800" windowWidth="24240" windowHeight="13140" xr2:uid="{2C62C16E-58CA-4B1E-8803-5541E16FBEAE}"/>
+    <workbookView xWindow="5080" yWindow="1540" windowWidth="24240" windowHeight="13140" xr2:uid="{2C62C16E-58CA-4B1E-8803-5541E16FBEAE}"/>
   </bookViews>
   <sheets>
     <sheet name="JCO" sheetId="6" r:id="rId1"/>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBBE860-1687-40CC-A910-F3F41CF7BB3F}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -603,9 +603,10 @@
     <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="54.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -665,8 +666,12 @@
       <c r="J2" t="s">
         <v>31</v>
       </c>
+      <c r="M2" t="str">
+        <f>(CONCATENATE("https://www.jacc.org/doi/",A2))</f>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2020.12.003</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -697,8 +702,12 @@
       <c r="J3" t="s">
         <v>33</v>
       </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M11" si="0">(CONCATENATE("https://www.jacc.org/doi/",A3))</f>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.05.006</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -729,8 +738,12 @@
       <c r="J4" t="s">
         <v>35</v>
       </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.07.008</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -761,8 +774,12 @@
       <c r="J5" t="s">
         <v>37</v>
       </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.03.001</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -793,8 +810,12 @@
       <c r="J6" t="s">
         <v>38</v>
       </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.06.007</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -825,8 +846,12 @@
       <c r="J7" t="s">
         <v>41</v>
       </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.06.003</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -857,8 +882,12 @@
       <c r="J8" t="s">
         <v>42</v>
       </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2020.11.012</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -889,8 +918,12 @@
       <c r="J9" t="s">
         <v>44</v>
       </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.01.011</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -921,8 +954,12 @@
       <c r="J10" t="s">
         <v>47</v>
       </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.06.005</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -952,6 +989,10 @@
       </c>
       <c r="J11" t="s">
         <v>48</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://www.jacc.org/doi/10.1016/j.jaccao.2021.07.005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>